<commit_message>
Fixing of alignment of excel generation rows and column Sheet1 and Sheet 2 update.
</commit_message>
<xml_diff>
--- a/planetary_positions.xlsx
+++ b/planetary_positions.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,101 +465,96 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Key</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Table 1</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Shreevathsa</t>
+          <t>09/09/1989</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10/05/1999</t>
+          <t>03:04:00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Time</t>
+          <t>Place</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>03:04:00</t>
+          <t>Puttur,Karnataka</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Place</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Puttur,Karnataka</t>
-        </is>
+          <t>Latitude</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>12.7632858</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Latitude</t>
+          <t>Longitude</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12.7632858</v>
+        <v>75.20184209999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Longitude</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>75.20184209999999</v>
+          <t>Timezone</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>tobefilled GMT+5.5</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Timezone</t>
+          <t>Sunrise</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>tobefilled GMT+5.5</t>
+          <t>tobefilled</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Sunrise</t>
+          <t>Sunset</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -571,7 +566,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Sunset</t>
+          <t>Ayanamsha</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -580,19 +575,10 @@
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Ayanamsha</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>tobefilled</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -693,17 +679,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Aries</t>
+          <t>Leo</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Bharani</t>
+          <t>Purva Phalguni</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -712,7 +698,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>24.96816340468312</v>
+        <v>142.4845860305107</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -746,26 +732,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Aquarius</t>
+          <t>Scorpio</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Saturn</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Shatabhisha</t>
+          <t>Jyeshtha</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Rahu</t>
+          <t>Mercury</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>309.075052640371</v>
+        <v>238.080245280088</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -783,7 +769,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -799,26 +785,26 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Aries</t>
+          <t>Virgo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>Mercury</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Ashwini</t>
+          <t>Hasta</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Ketu</t>
+          <t>Moon</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>7.96109256468479</v>
+        <v>166.4089687091878</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -836,7 +822,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -852,26 +838,26 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Gemini</t>
+          <t>Libra</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Mercury</t>
+          <t>Venus</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ardra</t>
+          <t>Chitra</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Rahu</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>67.50609350739118</v>
+        <v>182.0572724410369</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -905,35 +891,35 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Libra</t>
+          <t>Leo</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Venus</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Chitra</t>
+          <t>Uttara Phalguni</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>184.8265144931989</v>
+        <v>149.3837157754606</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Retro</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Combust</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -942,7 +928,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -958,26 +944,26 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pisces</t>
+          <t>Gemini</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Jupiter</t>
+          <t>Mercury</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Revati</t>
+          <t>Ardra</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Mercury</t>
+          <t>Rahu</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>356.3771724279898</v>
+        <v>73.33655250974485</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -995,7 +981,7 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -1011,17 +997,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Aries</t>
+          <t>Sagittarius</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>Jupiter</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Bharani</t>
+          <t>Purva Ashadha</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1030,16 +1016,16 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>14.49292394624836</v>
+        <v>253.590182561376</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Retro</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Combust</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1048,7 +1034,7 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -1064,30 +1050,30 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Capricorn</t>
+          <t>Sagittarius</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Saturn</t>
+          <t>Jupiter</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Shravana</t>
+          <t>Moola</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Moon</t>
+          <t>Ketu</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>292.8890339183791</v>
+        <v>247.622252771897</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Retro</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1101,7 +1087,7 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -1117,26 +1103,26 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Capricorn</t>
+          <t>Sagittarius</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Saturn</t>
+          <t>Jupiter</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Shravana</t>
+          <t>Purva Ashadha</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Moon</t>
+          <t>Venus</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>280.5216800641753</v>
+        <v>255.9345667638737</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1154,7 +1140,7 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -1170,30 +1156,30 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Scorpio</t>
+          <t>Libra</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>Venus</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Anuradha</t>
+          <t>Swati</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Saturn</t>
+          <t>Rahu</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>225.8449774019211</v>
+        <v>199.2862020569684</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Retro</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1207,7 +1193,7 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -1223,26 +1209,26 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Cancer</t>
+          <t>Aquarius</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Moon</t>
+          <t>Saturn</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ashlesha</t>
+          <t>Dhanishta</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Mercury</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>113.7254071935777</v>
+        <v>300.7872291398033</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1260,7 +1246,7 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -1276,30 +1262,30 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Capricorn</t>
+          <t>Leo</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Saturn</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Dhanishta</t>
+          <t>Magha</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>Ketu</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>293.560692356362</v>
+        <v>121.9004845901756</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Retro</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1313,7 +1299,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Succesful chart generation, reading by trigger script and db updation,avastha,status, ascendant nakshatra and nakshatra lord, sunrise sunset info ayanamsha to be fixed
</commit_message>
<xml_diff>
--- a/planetary_positions.xlsx
+++ b/planetary_positions.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,7 +479,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>09/09/1989</t>
+          <t>10/05/1999</t>
         </is>
       </c>
     </row>
@@ -503,7 +503,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Puttur,Karnataka</t>
+          <t>Bengaluru,India</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.7632858</v>
+        <v>12.98815675</v>
       </c>
     </row>
     <row r="6">
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>75.20184209999999</v>
+        <v>77.62260003796</v>
       </c>
     </row>
     <row r="7">
@@ -577,7 +577,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -679,17 +679,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Leo</t>
+          <t>Aries</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Purva Phalguni</t>
+          <t>Bharani</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>142.4845860305107</v>
+        <v>24.96816340468312</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -732,26 +732,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Scorpio</t>
+          <t>Aquarius</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>Saturn</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Jyeshtha</t>
+          <t>Shatabhisha</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Mercury</t>
+          <t>Rahu</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>238.080245280088</v>
+        <v>309.075052640371</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -769,7 +769,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -785,26 +785,26 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Virgo</t>
+          <t>Aries</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Mercury</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Hasta</t>
+          <t>Ashwini</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Moon</t>
+          <t>Ketu</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>166.4089687091878</v>
+        <v>7.96109256468479</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -838,26 +838,26 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Libra</t>
+          <t>Gemini</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Venus</t>
+          <t>Mercury</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Chitra</t>
+          <t>Ardra</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>Rahu</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>182.0572724410369</v>
+        <v>67.50609350739118</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -891,35 +891,35 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Leo</t>
+          <t>Libra</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Venus</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Uttara Phalguni</t>
+          <t>Chitra</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>149.3837157754606</v>
+        <v>184.8265144931989</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Retro</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Combust</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -928,7 +928,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -944,26 +944,26 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Gemini</t>
+          <t>Pisces</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Jupiter</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Revati</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Mercury</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Ardra</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Rahu</t>
-        </is>
-      </c>
       <c r="F8" t="n">
-        <v>73.33655250974485</v>
+        <v>356.3771724279898</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -981,7 +981,7 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -997,17 +997,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sagittarius</t>
+          <t>Aries</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Jupiter</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Purva Ashadha</t>
+          <t>Bharani</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1016,16 +1016,16 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>253.590182561376</v>
+        <v>14.49292394624836</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Retro</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Combust</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1034,7 +1034,7 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -1050,30 +1050,30 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sagittarius</t>
+          <t>Capricorn</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Jupiter</t>
+          <t>Saturn</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Moola</t>
+          <t>Shravana</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Ketu</t>
+          <t>Moon</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>247.622252771897</v>
+        <v>292.8890339183791</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Retro</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -1103,26 +1103,26 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sagittarius</t>
+          <t>Capricorn</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Jupiter</t>
+          <t>Saturn</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Purva Ashadha</t>
+          <t>Shravana</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Venus</t>
+          <t>Moon</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>255.9345667638737</v>
+        <v>280.5216800641753</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1140,7 +1140,7 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -1156,30 +1156,30 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Libra</t>
+          <t>Scorpio</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Venus</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Swati</t>
+          <t>Anuradha</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Rahu</t>
+          <t>Saturn</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>199.2862020569684</v>
+        <v>225.8449774019211</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Retro</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1193,7 +1193,7 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -1209,26 +1209,26 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Aquarius</t>
+          <t>Cancer</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Saturn</t>
+          <t>Moon</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Dhanishta</t>
+          <t>Ashlesha</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>Mercury</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>300.7872291398033</v>
+        <v>113.7254071935777</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1246,7 +1246,7 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -1262,30 +1262,30 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Leo</t>
+          <t>Capricorn</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Saturn</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Magha</t>
+          <t>Dhanishta</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Ketu</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>121.9004845901756</v>
+        <v>293.560692356362</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Retro</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1299,7 +1299,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>

</xml_diff>